<commit_message>
Making figures of spectrogram
Can make a figure of spectrogram
can also make spectrogram with CWT (wavelet toolbox).
</commit_message>
<xml_diff>
--- a/Control.xlsx
+++ b/Control.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Documents\ChangValiante2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA74588-A80D-4483-B48B-F4C7F77D0A5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C5C298-9E19-4E17-87F8-9CE8C09DC134}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="4680" windowWidth="38700" windowHeight="15435" activeTab="1" xr2:uid="{114BA0F1-3307-4066-A814-42B75BC19B5D}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="38700" windowHeight="15435" activeTab="5" xr2:uid="{3E8F6AD9-02D1-405C-A2FA-26D1B1067A03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="19812000" sheetId="2" r:id="rId2"/>
-    <sheet name="19815002" sheetId="3" r:id="rId3"/>
+    <sheet name="19n07003" sheetId="3" r:id="rId3"/>
+    <sheet name="19808006" sheetId="4" r:id="rId4"/>
+    <sheet name="19805005" sheetId="5" r:id="rId5"/>
+    <sheet name="19805000" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="42">
   <si>
     <t>Treatment Group</t>
   </si>
@@ -133,7 +136,34 @@
     <t>Multiple Comparison (Tukey-Kramer method), dominant frequency</t>
   </si>
   <si>
-    <t>HEPES(VGAT-ChR2)</t>
+    <t>Control(VGAT)</t>
+  </si>
+  <si>
+    <t>Control (Thy1)</t>
+  </si>
+  <si>
+    <t>Delay to Dominant Frequency, median</t>
+  </si>
+  <si>
+    <t>Delay to Dominant Frequency, IQR</t>
+  </si>
+  <si>
+    <t>Acidosis Control [pH 6.9]</t>
+  </si>
+  <si>
+    <t>one-way ANOVA, max dominant frequency</t>
+  </si>
+  <si>
+    <t>Multiple Comparison (Tukey-Kramer method), max dominant frequency</t>
+  </si>
+  <si>
+    <t>one-way ANOVA, delay to dominant frequency</t>
+  </si>
+  <si>
+    <t>Multiple Comparison (Tukey-Kramer method), delay to dominant frequency</t>
+  </si>
+  <si>
+    <t>HEPES(Thy1)</t>
   </si>
 </sst>
 </file>
@@ -484,7 +514,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9135B49-0A2C-420D-9733-BEC6794D41A6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36DB073D-01F6-4518-A823-EA57D07C3361}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -496,10 +526,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8479BA15-0CB3-4EAE-B914-79F102339AF7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F47C73CD-7B4F-4B85-A0C9-BB33CD50E66D}">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="A40" sqref="A40:F42"/>
     </sheetView>
   </sheetViews>
@@ -569,13 +599,13 @@
         <v>2.7279931259552415E-2</v>
       </c>
       <c r="I2">
-        <v>55.95068359375</v>
+        <v>15.328648325047128</v>
       </c>
       <c r="J2">
-        <v>15.25927734375</v>
+        <v>20.403304000735279</v>
       </c>
       <c r="K2">
-        <v>0.28035076026346795</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="L2">
         <v>23</v>
@@ -583,7 +613,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>26.859647999999652</v>
@@ -607,13 +637,13 @@
         <v>5.6066262743570405E-14</v>
       </c>
       <c r="I3">
-        <v>61.037109375</v>
+        <v>21.137914241166357</v>
       </c>
       <c r="J3">
-        <v>15.25927734375</v>
+        <v>3.9664796440514181</v>
       </c>
       <c r="K3">
-        <v>7.9550865602116355E-2</v>
+        <v>0.26620518062285592</v>
       </c>
       <c r="L3">
         <v>33</v>
@@ -645,13 +675,13 @@
         <v>1.3946154254762533E-6</v>
       </c>
       <c r="I4">
-        <v>71.2099609375</v>
+        <v>20.948782603859364</v>
       </c>
       <c r="J4">
-        <v>13.9876708984375</v>
+        <v>5.3621100133320994</v>
       </c>
       <c r="K4">
-        <v>9.5300240666551711E-2</v>
+        <v>0.57836994473302117</v>
       </c>
       <c r="L4">
         <v>11</v>
@@ -709,13 +739,13 @@
         <v>0.10144927536231885</v>
       </c>
       <c r="I6">
-        <v>0.40888849136492073</v>
+        <v>2.9562443506700713E-4</v>
       </c>
       <c r="J6">
-        <v>0.23188405797101447</v>
+        <v>0.54808959156785253</v>
       </c>
       <c r="K6">
-        <v>-0.21080368906455862</v>
+        <v>-0.1831357048748353</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1040,19 +1070,19 @@
         <v>23</v>
       </c>
       <c r="B34">
-        <v>963.51719247750771</v>
+        <v>65.866271720991222</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
       <c r="D34">
-        <v>481.75859623875385</v>
+        <v>32.933135860495611</v>
       </c>
       <c r="E34">
-        <v>4.7953934271893326</v>
+        <v>0.71439473998507763</v>
       </c>
       <c r="F34">
-        <v>1.1465919219038554E-2</v>
+        <v>0.49334966366205091</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1060,13 +1090,13 @@
         <v>24</v>
       </c>
       <c r="B35">
-        <v>6429.6184718574314</v>
+        <v>2950.3586422203298</v>
       </c>
       <c r="C35">
         <v>64</v>
       </c>
       <c r="D35">
-        <v>100.46278862277236</v>
+        <v>46.099353784692653</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1074,7 +1104,7 @@
         <v>25</v>
       </c>
       <c r="B36">
-        <v>7393.1356643349391</v>
+        <v>3016.2249139413211</v>
       </c>
       <c r="C36">
         <v>66</v>
@@ -1104,16 +1134,16 @@
         <v>2</v>
       </c>
       <c r="C40">
-        <v>-10.20496131478437</v>
+        <v>-2.7072812270902284</v>
       </c>
       <c r="D40">
-        <v>-3.6724128170289916</v>
+        <v>1.7178631712894976</v>
       </c>
       <c r="E40">
-        <v>2.8601356807263878</v>
+        <v>6.1430075696692237</v>
       </c>
       <c r="F40">
-        <v>0.3737803436591034</v>
+        <v>0.62254280640985105</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1124,16 +1154,16 @@
         <v>3</v>
       </c>
       <c r="C41">
-        <v>-20.19546635590978</v>
+        <v>-3.2824771159485255</v>
       </c>
       <c r="D41">
-        <v>-11.379118546195656</v>
+        <v>2.6897115540214145</v>
       </c>
       <c r="E41">
-        <v>-2.5627707364815304</v>
+        <v>8.6619002239913545</v>
       </c>
       <c r="F41">
-        <v>8.0575169962183724E-3</v>
+        <v>0.52946686417634214</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1144,16 +1174,16 @@
         <v>3</v>
       </c>
       <c r="C42">
-        <v>-16.079733715065789</v>
+        <v>-4.7000357069169274</v>
       </c>
       <c r="D42">
-        <v>-7.7067057291666643</v>
+        <v>0.97184838273191687</v>
       </c>
       <c r="E42">
-        <v>0.66632225673246026</v>
+        <v>6.6437324723807611</v>
       </c>
       <c r="F42">
-        <v>7.7371039529495089E-2</v>
+        <v>0.91117527722382963</v>
       </c>
     </row>
   </sheetData>
@@ -1162,10 +1192,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF522182-F29D-4DA0-A943-BB84FB3EEE7E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6547055A-54E1-4734-9ECF-6C7447E300AA}">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="A40" sqref="A40:F42"/>
     </sheetView>
   </sheetViews>
@@ -1214,75 +1244,75 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>20.954304000000093</v>
+        <v>28.100962500000151</v>
       </c>
       <c r="C2">
-        <v>4.4960400000002778</v>
+        <v>11.147711249999972</v>
       </c>
       <c r="D2">
-        <v>0.83481278656757951</v>
+        <v>5.0509980645571551E-2</v>
       </c>
       <c r="E2">
-        <v>709711.54916757869</v>
+        <v>97213.707610082885</v>
       </c>
       <c r="F2">
-        <v>91376.400962436688</v>
+        <v>43321.411971868481</v>
       </c>
       <c r="G2">
-        <v>0.57709011825478551</v>
+        <v>8.636138863723121E-2</v>
       </c>
       <c r="H2">
-        <v>1.5135674130029031E-5</v>
+        <v>2.7537019651074246E-2</v>
       </c>
       <c r="I2">
-        <v>27.33953857421875</v>
+        <v>10.133862836875752</v>
       </c>
       <c r="J2">
-        <v>3.9737701416015625</v>
+        <v>2.3035036451195126</v>
       </c>
       <c r="K2">
-        <v>5.0000000000000001E-4</v>
+        <v>4.3586802338778555E-2</v>
       </c>
       <c r="L2">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B3">
-        <v>108.70166400000016</v>
+        <v>25.35151124999993</v>
       </c>
       <c r="C3">
-        <v>46.819439999999986</v>
+        <v>3.992283750000297</v>
       </c>
       <c r="D3">
-        <v>0.4914594933762596</v>
+        <v>0.28439820728453324</v>
       </c>
       <c r="E3">
-        <v>229772.86715790053</v>
+        <v>79308.60936802678</v>
       </c>
       <c r="F3">
-        <v>65184.581893080584</v>
+        <v>31645.117423461998</v>
       </c>
       <c r="G3">
-        <v>2.264149358508299E-3</v>
+        <v>0.49329283551135295</v>
       </c>
       <c r="H3">
-        <v>0.67864172233188191</v>
+        <v>4.5826322792041907E-7</v>
       </c>
       <c r="I3">
-        <v>45.77783203125</v>
+        <v>9.0082442187708374</v>
       </c>
       <c r="J3">
-        <v>33.856521606445313</v>
+        <v>2.1567759139458804</v>
       </c>
       <c r="K3">
-        <v>1.1895345992301088E-2</v>
+        <v>0.44210725272159362</v>
       </c>
       <c r="L3">
-        <v>17</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1290,37 +1320,37 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <v>26.711040000000594</v>
+        <v>21.068531249999978</v>
       </c>
       <c r="C4">
-        <v>3.7341119999991861</v>
+        <v>6.5151449999993929</v>
       </c>
       <c r="D4">
-        <v>0.52378414335727796</v>
+        <v>0.27510070894586952</v>
       </c>
       <c r="E4">
-        <v>814138.73210176313</v>
+        <v>92892.088734417674</v>
       </c>
       <c r="F4">
-        <v>93776.87935968698</v>
+        <v>33103.020431348792</v>
       </c>
       <c r="G4">
-        <v>0.98362373116120183</v>
+        <v>0.49479406239598217</v>
       </c>
       <c r="H4">
-        <v>7.1108833465172161E-4</v>
+        <v>3.1414758572267942E-7</v>
       </c>
       <c r="I4">
-        <v>22.571014404296875</v>
+        <v>8.1035023713106149</v>
       </c>
       <c r="J4">
-        <v>8.9012451171875</v>
+        <v>1.7751470649623338</v>
       </c>
       <c r="K4">
-        <v>0.26692673382429599</v>
+        <v>0.14781360891041403</v>
       </c>
       <c r="L4">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1357,31 +1387,31 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>5.5889117092916095E-7</v>
+        <v>5.4184566780015771E-2</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0.32999999999999996</v>
       </c>
       <c r="D6">
-        <v>-1</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="E6">
-        <v>5.5889117092916095E-7</v>
+        <v>1.4722119027441119E-2</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0.38499999999999995</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0.38600000000000001</v>
       </c>
       <c r="I6">
-        <v>2.9119084212550293E-2</v>
+        <v>3.4527781281233572E-2</v>
       </c>
       <c r="J6">
-        <v>0.52941176470588236</v>
+        <v>0.35</v>
       </c>
       <c r="K6">
-        <v>-0.32620320855614976</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1414,19 +1444,19 @@
         <v>23</v>
       </c>
       <c r="B10">
-        <v>68614.561667469345</v>
+        <v>527.36941652710152</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10">
-        <v>34307.280833734672</v>
+        <v>263.68470826355076</v>
       </c>
       <c r="E10">
-        <v>88.224107769843613</v>
+        <v>8.2970783930478422</v>
       </c>
       <c r="F10">
-        <v>5.7242031987585656E-14</v>
+        <v>5.3157586207690471E-4</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1434,13 +1464,13 @@
         <v>24</v>
       </c>
       <c r="B11">
-        <v>12832.549924638937</v>
+        <v>2542.4342957587896</v>
       </c>
       <c r="C11">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="D11">
-        <v>388.86514923148297</v>
+        <v>31.78042869698487</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1448,10 +1478,10 @@
         <v>25</v>
       </c>
       <c r="B12">
-        <v>81447.111592108282</v>
+        <v>3069.8037122858909</v>
       </c>
       <c r="C12">
-        <v>35</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1478,16 +1508,16 @@
         <v>2</v>
       </c>
       <c r="C16">
-        <v>-107.88156006610389</v>
+        <v>-0.98459748128090752</v>
       </c>
       <c r="D16">
-        <v>-89.157675283422492</v>
+        <v>2.4477382875000657</v>
       </c>
       <c r="E16">
-        <v>-70.433790500741097</v>
+        <v>5.880074056281039</v>
       </c>
       <c r="F16">
-        <v>9.5805785527147691E-10</v>
+        <v>0.2103492123343258</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1498,16 +1528,16 @@
         <v>3</v>
       </c>
       <c r="C17">
-        <v>-26.662966761198479</v>
+        <v>2.9010155520693628</v>
       </c>
       <c r="D17">
-        <v>-4.1789856363642244</v>
+        <v>7.0626224888888771</v>
       </c>
       <c r="E17">
-        <v>18.304995488470031</v>
+        <v>11.224229425708391</v>
       </c>
       <c r="F17">
-        <v>0.89205331000165278</v>
+        <v>3.4010620670044123E-4</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1518,16 +1548,16 @@
         <v>3</v>
       </c>
       <c r="C18">
-        <v>64.232502188289487</v>
+        <v>0.79385077928712011</v>
       </c>
       <c r="D18">
-        <v>84.978689647058275</v>
+        <v>4.6148842013888114</v>
       </c>
       <c r="E18">
-        <v>105.72487710582706</v>
+        <v>8.4359176234905036</v>
       </c>
       <c r="F18">
-        <v>9.9965657973655198E-10</v>
+        <v>1.3814118036645118E-2</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1560,19 +1590,19 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <v>2446809733137.2139</v>
+        <v>6299342204.5513382</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22">
-        <v>1223404866568.6069</v>
+        <v>3149671102.2756691</v>
       </c>
       <c r="E22">
-        <v>179.85783121012724</v>
+        <v>4.7832411723932164</v>
       </c>
       <c r="F22">
-        <v>1.7913866776476244E-18</v>
+        <v>1.0908844749133083E-2</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1580,13 +1610,13 @@
         <v>24</v>
       </c>
       <c r="B23">
-        <v>224468183148.48438</v>
+        <v>52678441061.332184</v>
       </c>
       <c r="C23">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="D23">
-        <v>6802066156.014678</v>
+        <v>658480513.26665235</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1594,10 +1624,10 @@
         <v>25</v>
       </c>
       <c r="B24">
-        <v>2671277916285.6982</v>
+        <v>58977783265.883522</v>
       </c>
       <c r="C24">
-        <v>35</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1624,16 +1654,16 @@
         <v>2</v>
       </c>
       <c r="C28">
-        <v>394840.7928014872</v>
+        <v>4257.2829668001687</v>
       </c>
       <c r="D28">
-        <v>473150.729779171</v>
+        <v>19880.891696599007</v>
       </c>
       <c r="E28">
-        <v>551460.66675685486</v>
+        <v>35504.500426397848</v>
       </c>
       <c r="F28">
-        <v>9.5720886772454605E-10</v>
+        <v>8.9072401668018886E-3</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1644,16 +1674,16 @@
         <v>3</v>
       </c>
       <c r="C29">
-        <v>-197849.67314929765</v>
+        <v>-10646.510413126369</v>
       </c>
       <c r="D29">
-        <v>-103813.67766390694</v>
+        <v>8296.6591507234407</v>
       </c>
       <c r="E29">
-        <v>-9777.6821785162465</v>
+        <v>27239.82871457325</v>
       </c>
       <c r="F29">
-        <v>2.7904493271711073E-2</v>
+        <v>0.55031155331944415</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1664,16 +1694,16 @@
         <v>3</v>
       </c>
       <c r="C30">
-        <v>-663732.33254407509</v>
+        <v>-28977.149542339332</v>
       </c>
       <c r="D30">
-        <v>-576964.407443078</v>
+        <v>-11584.232545875566</v>
       </c>
       <c r="E30">
-        <v>-490196.48234208091</v>
+        <v>5808.6844505882</v>
       </c>
       <c r="F30">
-        <v>9.5720764647921897E-10</v>
+        <v>0.25560838298452859</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1706,19 +1736,19 @@
         <v>23</v>
       </c>
       <c r="B34">
-        <v>2117.7626259640019</v>
+        <v>22.063799943515743</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
       <c r="D34">
-        <v>1058.881312982001</v>
+        <v>11.031899971757872</v>
       </c>
       <c r="E34">
-        <v>5.1422046403078454</v>
+        <v>3.5325883568853165</v>
       </c>
       <c r="F34">
-        <v>1.1376543769456694E-2</v>
+        <v>3.3870378224426352E-2</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1726,13 +1756,13 @@
         <v>24</v>
       </c>
       <c r="B35">
-        <v>6795.3505884421811</v>
+        <v>249.83154236481033</v>
       </c>
       <c r="C35">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="D35">
-        <v>205.91971480127822</v>
+        <v>3.1228942795601293</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1740,10 +1770,10 @@
         <v>25</v>
       </c>
       <c r="B36">
-        <v>8913.113214406183</v>
+        <v>271.89534230832606</v>
       </c>
       <c r="C36">
-        <v>35</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1770,16 +1800,16 @@
         <v>2</v>
       </c>
       <c r="C40">
-        <v>-28.204553173118303</v>
+        <v>-0.44664785314402211</v>
       </c>
       <c r="D40">
-        <v>-14.579273897058822</v>
+        <v>0.62929333141818589</v>
       </c>
       <c r="E40">
-        <v>-0.9539946209993424</v>
+        <v>1.7052345159803939</v>
       </c>
       <c r="F40">
-        <v>3.3891517982837294E-2</v>
+        <v>0.34743460182087715</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1790,16 +1820,16 @@
         <v>3</v>
       </c>
       <c r="C41">
-        <v>-14.620249147490583</v>
+        <v>0.14713928199866144</v>
       </c>
       <c r="D41">
-        <v>1.7412338256835973</v>
+        <v>1.4516865637682912</v>
       </c>
       <c r="E41">
-        <v>18.102716798857777</v>
+        <v>2.7562338455379209</v>
       </c>
       <c r="F41">
-        <v>0.96314744825116627</v>
+        <v>2.5470371041809492E-2</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1810,16 +1840,2566 @@
         <v>3</v>
       </c>
       <c r="C42">
-        <v>1.223608691369142</v>
+        <v>-0.37539378598930839</v>
       </c>
       <c r="D42">
-        <v>16.32050772274242</v>
+        <v>0.82239323235010531</v>
       </c>
       <c r="E42">
-        <v>31.417406754115696</v>
+        <v>2.0201802506895188</v>
       </c>
       <c r="F42">
-        <v>3.1830083281166655E-2</v>
+        <v>0.23511528296590023</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6733BB35-19C0-4DAA-A782-F055810F40EE}">
+  <dimension ref="A1:O54"/>
+  <sheetViews>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:F54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>34.902719999999988</v>
+      </c>
+      <c r="C2">
+        <v>4.2633599999999774</v>
+      </c>
+      <c r="D2">
+        <v>0.13592920520087134</v>
+      </c>
+      <c r="E2">
+        <v>333066.18185236154</v>
+      </c>
+      <c r="F2">
+        <v>100029.89335731574</v>
+      </c>
+      <c r="G2">
+        <v>0.96069017716404392</v>
+      </c>
+      <c r="H2">
+        <v>2.3388695598475229E-3</v>
+      </c>
+      <c r="I2">
+        <v>16.797558740410231</v>
+      </c>
+      <c r="J2">
+        <v>2.1322170890448078</v>
+      </c>
+      <c r="K2">
+        <v>0.57925824802504133</v>
+      </c>
+      <c r="L2">
+        <v>7.0018239416338659</v>
+      </c>
+      <c r="M2">
+        <v>12.503599884803684</v>
+      </c>
+      <c r="N2">
+        <v>9.6585029436668815E-2</v>
+      </c>
+      <c r="O2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3">
+        <v>50.079263999999966</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>107650.6315092445</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0.91507869733584324</v>
+      </c>
+      <c r="I3">
+        <v>23.992688860687242</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>2.5005279831045359</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>38.129183999999441</v>
+      </c>
+      <c r="C4">
+        <v>5.2088399999995545</v>
+      </c>
+      <c r="E4">
+        <v>526265.32666424965</v>
+      </c>
+      <c r="F4">
+        <v>31230.904392603668</v>
+      </c>
+      <c r="H4">
+        <v>4.7728568118042158E-2</v>
+      </c>
+      <c r="I4">
+        <v>22.475756665115568</v>
+      </c>
+      <c r="J4">
+        <v>6.4461282308909595</v>
+      </c>
+      <c r="L4">
+        <v>3.5008159738888365</v>
+      </c>
+      <c r="M4">
+        <v>3.7510799654411047</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>0.15036559272503558</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>-1</v>
+      </c>
+      <c r="E6">
+        <v>0.15036559272503558</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0.15036559272503558</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>-1</v>
+      </c>
+      <c r="L6">
+        <v>0.15036559272503558</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>156.1683649923834</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>78.084182496191701</v>
+      </c>
+      <c r="E10">
+        <v>6.7250940138589783</v>
+      </c>
+      <c r="F10">
+        <v>3.82316480643781E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <v>58.054342686717035</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>11.610868537343407</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>214.22270767910044</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>-26.368075489480873</v>
+      </c>
+      <c r="D16">
+        <v>-13.971743999999973</v>
+      </c>
+      <c r="E16">
+        <v>-1.5754125105190742</v>
+      </c>
+      <c r="F16">
+        <v>3.2485281787097087E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>-11.281426563415001</v>
+      </c>
+      <c r="D17">
+        <v>-2.8131199999999765</v>
+      </c>
+      <c r="E17">
+        <v>5.6551865634150484</v>
+      </c>
+      <c r="F17">
+        <v>0.56452295063874325</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>-1.6442521100869634</v>
+      </c>
+      <c r="D18">
+        <v>11.158623999999996</v>
+      </c>
+      <c r="E18">
+        <v>23.961500110086956</v>
+      </c>
+      <c r="F18">
+        <v>7.9059877992322058E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>144374623149.68661</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>72187311574.843307</v>
+      </c>
+      <c r="E22">
+        <v>27.02277041925468</v>
+      </c>
+      <c r="F22">
+        <v>2.0866867022578612E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <v>13356756256.828369</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>2671351251.365674</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24">
+        <v>157731379406.51498</v>
+      </c>
+      <c r="C24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>40235.999726392445</v>
+      </c>
+      <c r="D28">
+        <v>228265.64444393129</v>
+      </c>
+      <c r="E28">
+        <v>416295.28916147014</v>
+      </c>
+      <c r="F28">
+        <v>2.4513565615428945E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>-316821.73523570056</v>
+      </c>
+      <c r="D29">
+        <v>-188373.03443826752</v>
+      </c>
+      <c r="E29">
+        <v>-59924.333640834491</v>
+      </c>
+      <c r="F29">
+        <v>1.1483921954874687E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>-610834.86090468557</v>
+      </c>
+      <c r="D30">
+        <v>-416638.67888219882</v>
+      </c>
+      <c r="E30">
+        <v>-222442.49685971209</v>
+      </c>
+      <c r="F30">
+        <v>2.16953466762837E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34">
+        <v>100.47103912396796</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>50.235519561983978</v>
+      </c>
+      <c r="E34">
+        <v>5.0830951974513878</v>
+      </c>
+      <c r="F34">
+        <v>6.2407064019746383E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35">
+        <v>49.414301336685128</v>
+      </c>
+      <c r="C35">
+        <v>5</v>
+      </c>
+      <c r="D35">
+        <v>9.8828602673370263</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36">
+        <v>149.88534046065308</v>
+      </c>
+      <c r="C36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" t="s">
+        <v>27</v>
+      </c>
+      <c r="F39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>-18.331702239151959</v>
+      </c>
+      <c r="D40">
+        <v>-6.8949646974995673</v>
+      </c>
+      <c r="E40">
+        <v>4.541772844152824</v>
+      </c>
+      <c r="F40">
+        <v>0.21666457135995154</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>-14.962438487353067</v>
+      </c>
+      <c r="D41">
+        <v>-7.1496593865188096</v>
+      </c>
+      <c r="E41">
+        <v>0.66311971431544769</v>
+      </c>
+      <c r="F41">
+        <v>6.7523096306497443E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <v>-12.06650643135654</v>
+      </c>
+      <c r="D42">
+        <v>-0.2546946890192423</v>
+      </c>
+      <c r="E42">
+        <v>11.557117053318056</v>
+      </c>
+      <c r="F42">
+        <v>0.9972910668245708</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" t="s">
+        <v>21</v>
+      </c>
+      <c r="F45" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46">
+        <v>106.51966020067098</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>53.259830100335492</v>
+      </c>
+      <c r="E46">
+        <v>0.94573586023097456</v>
+      </c>
+      <c r="F46">
+        <v>0.44837879448017604</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47">
+        <v>281.57878082009063</v>
+      </c>
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <v>56.315756164018126</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48">
+        <v>388.09844102076164</v>
+      </c>
+      <c r="C48">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>27</v>
+      </c>
+      <c r="B51" t="s">
+        <v>27</v>
+      </c>
+      <c r="F51" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <v>-19.048450084581642</v>
+      </c>
+      <c r="D52">
+        <v>8.2523759239704333</v>
+      </c>
+      <c r="E52">
+        <v>35.553201932522512</v>
+      </c>
+      <c r="F52">
+        <v>0.61727560888912625</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <v>-11.731356062386123</v>
+      </c>
+      <c r="D53">
+        <v>6.9186586029247037</v>
+      </c>
+      <c r="E53">
+        <v>25.568673268235532</v>
+      </c>
+      <c r="F53">
+        <v>0.49923278144705308</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>2</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="C54">
+        <v>-29.529889179399994</v>
+      </c>
+      <c r="D54">
+        <v>-1.3337173210457305</v>
+      </c>
+      <c r="E54">
+        <v>26.862454537308537</v>
+      </c>
+      <c r="F54">
+        <v>0.98705857657208962</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A557DD0-B9BB-452C-B7D5-D2B64CEEAB29}">
+  <dimension ref="A1:O54"/>
+  <sheetViews>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:F54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>48.82195200000001</v>
+      </c>
+      <c r="C2">
+        <v>10.546967999999993</v>
+      </c>
+      <c r="D2">
+        <v>0.3567518330505744</v>
+      </c>
+      <c r="E2">
+        <v>100.96481370723454</v>
+      </c>
+      <c r="F2">
+        <v>112.2706804858058</v>
+      </c>
+      <c r="G2">
+        <v>0.53414541382916458</v>
+      </c>
+      <c r="H2">
+        <v>5.6024136040194739E-3</v>
+      </c>
+      <c r="I2">
+        <v>5.7917679589661555</v>
+      </c>
+      <c r="J2">
+        <v>0.74312653026952802</v>
+      </c>
+      <c r="K2">
+        <v>0.36426332220709412</v>
+      </c>
+      <c r="L2">
+        <v>24.506863780359019</v>
+      </c>
+      <c r="M2">
+        <v>15.004319861764426</v>
+      </c>
+      <c r="N2">
+        <v>0.80403831077362953</v>
+      </c>
+      <c r="O2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3">
+        <v>76.341886000000159</v>
+      </c>
+      <c r="C3">
+        <v>24.721825999999965</v>
+      </c>
+      <c r="D3">
+        <v>7.1925815254022793E-2</v>
+      </c>
+      <c r="E3">
+        <v>2.9762890253031076</v>
+      </c>
+      <c r="F3">
+        <v>2.7769561133804044</v>
+      </c>
+      <c r="G3">
+        <v>0.75793171394834902</v>
+      </c>
+      <c r="H3">
+        <v>1.5901494048599862E-2</v>
+      </c>
+      <c r="I3">
+        <v>10.055368442820859</v>
+      </c>
+      <c r="J3">
+        <v>2.1905443858683462</v>
+      </c>
+      <c r="K3">
+        <v>0.54657038567247918</v>
+      </c>
+      <c r="L3">
+        <v>52.014783526927133</v>
+      </c>
+      <c r="M3">
+        <v>14.004031870980114</v>
+      </c>
+      <c r="N3">
+        <v>9.357195727143125E-2</v>
+      </c>
+      <c r="O3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>25.214109999998982</v>
+      </c>
+      <c r="C4">
+        <v>7.0914210000005369</v>
+      </c>
+      <c r="E4">
+        <v>2.3311279492620427</v>
+      </c>
+      <c r="F4">
+        <v>2.4466664498981565</v>
+      </c>
+      <c r="H4">
+        <v>1.4544759862259782E-2</v>
+      </c>
+      <c r="I4">
+        <v>10.794286159349543</v>
+      </c>
+      <c r="J4">
+        <v>5.8114679605217017</v>
+      </c>
+      <c r="L4">
+        <v>9.5025439185946023</v>
+      </c>
+      <c r="M4">
+        <v>5.2515119516175428</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>7.9527283115616491E-4</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>-1</v>
+      </c>
+      <c r="E6">
+        <v>7.9527283115616491E-4</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>7.9527283115616491E-4</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>-1</v>
+      </c>
+      <c r="L6">
+        <v>3.6818936524786815E-2</v>
+      </c>
+      <c r="M6">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="N6">
+        <v>-0.8571428571428571</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>8241.0399747109768</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>4120.5199873554884</v>
+      </c>
+      <c r="E10">
+        <v>10.422409324913911</v>
+      </c>
+      <c r="F10">
+        <v>1.9903641749786406E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <v>5139.57552094739</v>
+      </c>
+      <c r="C11">
+        <v>13</v>
+      </c>
+      <c r="D11">
+        <v>395.35196314979925</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>13380.615495658367</v>
+      </c>
+      <c r="C12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>-68.141813489011724</v>
+      </c>
+      <c r="D16">
+        <v>-38.932939428571572</v>
+      </c>
+      <c r="E16">
+        <v>-9.7240653681314271</v>
+      </c>
+      <c r="F16">
+        <v>9.8198191374104793E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>-17.159481512600699</v>
+      </c>
+      <c r="D17">
+        <v>19.069667904762383</v>
+      </c>
+      <c r="E17">
+        <v>55.298817322125466</v>
+      </c>
+      <c r="F17">
+        <v>0.37433512144356096</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>20.878776296102615</v>
+      </c>
+      <c r="D18">
+        <v>58.002607333333955</v>
+      </c>
+      <c r="E18">
+        <v>95.126438370565296</v>
+      </c>
+      <c r="F18">
+        <v>3.1860685962358248E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>55358.987393813448</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>27679.493696906724</v>
+      </c>
+      <c r="E22">
+        <v>12.644056832913581</v>
+      </c>
+      <c r="F22">
+        <v>8.9272147338677939E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <v>28458.69983145834</v>
+      </c>
+      <c r="C23">
+        <v>13</v>
+      </c>
+      <c r="D23">
+        <v>2189.1307562660263</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24">
+        <v>83817.687225271788</v>
+      </c>
+      <c r="C24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>49.921794129761366</v>
+      </c>
+      <c r="D28">
+        <v>118.65375238765749</v>
+      </c>
+      <c r="E28">
+        <v>187.38571064555362</v>
+      </c>
+      <c r="F28">
+        <v>1.4490423518445095E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>33.157953037064914</v>
+      </c>
+      <c r="D29">
+        <v>118.4094550402119</v>
+      </c>
+      <c r="E29">
+        <v>203.66095704335888</v>
+      </c>
+      <c r="F29">
+        <v>7.4493903640476811E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>-87.60109172248093</v>
+      </c>
+      <c r="D30">
+        <v>-0.2442973474456025</v>
+      </c>
+      <c r="E30">
+        <v>87.11249702758974</v>
+      </c>
+      <c r="F30">
+        <v>0.99996993930889078</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34">
+        <v>75.442188819349184</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>37.721094409674592</v>
+      </c>
+      <c r="E34">
+        <v>8.9785558924548319</v>
+      </c>
+      <c r="F34">
+        <v>3.5537670793709419E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35">
+        <v>54.616158010204941</v>
+      </c>
+      <c r="C35">
+        <v>13</v>
+      </c>
+      <c r="D35">
+        <v>4.2012429238619182</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36">
+        <v>130.05834682955413</v>
+      </c>
+      <c r="C36">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" t="s">
+        <v>27</v>
+      </c>
+      <c r="F39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>-7.6946109612840328</v>
+      </c>
+      <c r="D40">
+        <v>-4.6836039739101967</v>
+      </c>
+      <c r="E40">
+        <v>-1.672596986536361</v>
+      </c>
+      <c r="F40">
+        <v>3.2949390720764526E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>-7.2658515620785007</v>
+      </c>
+      <c r="D41">
+        <v>-3.5311570368268423</v>
+      </c>
+      <c r="E41">
+        <v>0.20353748842481645</v>
+      </c>
+      <c r="F41">
+        <v>6.4727219448888262E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <v>-2.6744761555319059</v>
+      </c>
+      <c r="D42">
+        <v>1.1524469370833543</v>
+      </c>
+      <c r="E42">
+        <v>4.9793700296986145</v>
+      </c>
+      <c r="F42">
+        <v>0.71242768840999071</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" t="s">
+        <v>21</v>
+      </c>
+      <c r="F45" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46">
+        <v>3486.5072967756219</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>1743.2536483878109</v>
+      </c>
+      <c r="E46">
+        <v>16.56252285191956</v>
+      </c>
+      <c r="F46">
+        <v>2.6609856239594664E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47">
+        <v>1368.2877682137073</v>
+      </c>
+      <c r="C47">
+        <v>13</v>
+      </c>
+      <c r="D47">
+        <v>105.25290524720825</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48">
+        <v>4854.7950649893291</v>
+      </c>
+      <c r="C48">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>27</v>
+      </c>
+      <c r="B51" t="s">
+        <v>27</v>
+      </c>
+      <c r="F51" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <v>-37.243975597893062</v>
+      </c>
+      <c r="D52">
+        <v>-22.173050462385199</v>
+      </c>
+      <c r="E52">
+        <v>-7.1021253268773368</v>
+      </c>
+      <c r="F52">
+        <v>4.9711901490619992E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <v>-1.0214274881096088</v>
+      </c>
+      <c r="D53">
+        <v>17.671754503855873</v>
+      </c>
+      <c r="E53">
+        <v>36.364936495821354</v>
+      </c>
+      <c r="F53">
+        <v>6.4770607294871496E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>2</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="C54">
+        <v>20.689993413161787</v>
+      </c>
+      <c r="D54">
+        <v>39.844804966241071</v>
+      </c>
+      <c r="E54">
+        <v>58.999616519320355</v>
+      </c>
+      <c r="F54">
+        <v>2.8402281926254158E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{553B1189-8259-4161-9C71-107DE1B79ABB}">
+  <dimension ref="A1:O54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:F54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>12.899535000000014</v>
+      </c>
+      <c r="C2">
+        <v>5.1831359999998767</v>
+      </c>
+      <c r="D2">
+        <v>0.44277954654598434</v>
+      </c>
+      <c r="E2">
+        <v>295335.53033840557</v>
+      </c>
+      <c r="F2">
+        <v>130103.23326148576</v>
+      </c>
+      <c r="G2">
+        <v>0.7953557290967066</v>
+      </c>
+      <c r="H2">
+        <v>0.20543240654644268</v>
+      </c>
+      <c r="I2">
+        <v>12.954748861160326</v>
+      </c>
+      <c r="J2">
+        <v>3.8633442555293591</v>
+      </c>
+      <c r="K2">
+        <v>0.28615238456162917</v>
+      </c>
+      <c r="L2">
+        <v>2.5005279831045359</v>
+      </c>
+      <c r="M2">
+        <v>1.0002879907842908</v>
+      </c>
+      <c r="N2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="O2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3">
+        <v>63.321023999999852</v>
+      </c>
+      <c r="C3">
+        <v>87.460271999999918</v>
+      </c>
+      <c r="E3">
+        <v>130799.00983475964</v>
+      </c>
+      <c r="F3">
+        <v>116988.38552699925</v>
+      </c>
+      <c r="H3">
+        <v>7.1529707079602822E-3</v>
+      </c>
+      <c r="I3">
+        <v>12.256874079792482</v>
+      </c>
+      <c r="J3">
+        <v>0.94509743715460104</v>
+      </c>
+      <c r="L3">
+        <v>18.50513583565326</v>
+      </c>
+      <c r="M3">
+        <v>18.75539982720553</v>
+      </c>
+      <c r="O3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>21.63110400000005</v>
+      </c>
+      <c r="C4">
+        <v>3.5627520000005006</v>
+      </c>
+      <c r="D4">
+        <v>0.85073937132170852</v>
+      </c>
+      <c r="E4">
+        <v>69455.789809561044</v>
+      </c>
+      <c r="F4">
+        <v>4907.3794468311535</v>
+      </c>
+      <c r="G4">
+        <v>0.61070674819711923</v>
+      </c>
+      <c r="H4">
+        <v>7.8273477437384997E-4</v>
+      </c>
+      <c r="I4">
+        <v>10.211381928638835</v>
+      </c>
+      <c r="J4">
+        <v>1.4425964247530931</v>
+      </c>
+      <c r="K4">
+        <v>9.3725478970695095E-2</v>
+      </c>
+      <c r="L4">
+        <v>1.5002399923202452</v>
+      </c>
+      <c r="M4">
+        <v>4.5012959585293286</v>
+      </c>
+      <c r="N4">
+        <v>3.7804766628877755E-3</v>
+      </c>
+      <c r="O4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>4.0271940537589179E-3</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>-1</v>
+      </c>
+      <c r="E6">
+        <v>8.4231268882156832E-2</v>
+      </c>
+      <c r="F6">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="G6">
+        <v>0.76190476190476186</v>
+      </c>
+      <c r="I6">
+        <v>0.41964005973286056</v>
+      </c>
+      <c r="J6">
+        <v>0.5</v>
+      </c>
+      <c r="K6">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="L6">
+        <v>0.12667331546420513</v>
+      </c>
+      <c r="M6">
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="N6">
+        <v>-0.47619047619047616</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>14717.600058573662</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>7358.800029286831</v>
+      </c>
+      <c r="E10">
+        <v>17.274878357743596</v>
+      </c>
+      <c r="F10">
+        <v>5.3083914258542326E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <v>8093.6720746155443</v>
+      </c>
+      <c r="C11">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>425.98274076923917</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>22811.272133189206</v>
+      </c>
+      <c r="C12">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>-110.33787295131245</v>
+      </c>
+      <c r="D16">
+        <v>-76.979373714285458</v>
+      </c>
+      <c r="E16">
+        <v>-43.620874477258461</v>
+      </c>
+      <c r="F16">
+        <v>3.4436812084148727E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>-36.427921943223147</v>
+      </c>
+      <c r="D17">
+        <v>-9.1108297142856269</v>
+      </c>
+      <c r="E17">
+        <v>18.20626251465189</v>
+      </c>
+      <c r="F17">
+        <v>0.67897267276997586</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>29.576720146730459</v>
+      </c>
+      <c r="D18">
+        <v>67.868543999999844</v>
+      </c>
+      <c r="E18">
+        <v>106.16036785326924</v>
+      </c>
+      <c r="F18">
+        <v>6.8127288478725401E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>216124066885.70807</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>108062033442.85403</v>
+      </c>
+      <c r="E22">
+        <v>18.059751020481485</v>
+      </c>
+      <c r="F22">
+        <v>4.0342146066826638E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <v>113688091994.49792</v>
+      </c>
+      <c r="C23">
+        <v>19</v>
+      </c>
+      <c r="D23">
+        <v>5983583789.1841011</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24">
+        <v>329812158880.20599</v>
+      </c>
+      <c r="C24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>12659.07944303524</v>
+      </c>
+      <c r="D28">
+        <v>137682.44644055775</v>
+      </c>
+      <c r="E28">
+        <v>262705.81343808025</v>
+      </c>
+      <c r="F28">
+        <v>2.9505950372525236E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>131239.5218684373</v>
+      </c>
+      <c r="D29">
+        <v>233620.47200580934</v>
+      </c>
+      <c r="E29">
+        <v>336001.42214318138</v>
+      </c>
+      <c r="F29">
+        <v>3.9595074869946956E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>-47574.807928706519</v>
+      </c>
+      <c r="D30">
+        <v>95938.025565251592</v>
+      </c>
+      <c r="E30">
+        <v>239450.8590592097</v>
+      </c>
+      <c r="F30">
+        <v>0.23161489327003182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34">
+        <v>38.112335341685309</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>19.056167670842655</v>
+      </c>
+      <c r="E34">
+        <v>4.5915494790939713</v>
+      </c>
+      <c r="F34">
+        <v>2.3619251259144144E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35">
+        <v>78.855120127651432</v>
+      </c>
+      <c r="C35">
+        <v>19</v>
+      </c>
+      <c r="D35">
+        <v>4.1502694804027067</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36">
+        <v>116.96745546933674</v>
+      </c>
+      <c r="C36">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" t="s">
+        <v>27</v>
+      </c>
+      <c r="F39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>-2.3898485745075444</v>
+      </c>
+      <c r="D40">
+        <v>0.90282479044762454</v>
+      </c>
+      <c r="E40">
+        <v>4.1954981554027935</v>
+      </c>
+      <c r="F40">
+        <v>0.76833525375823775</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>0.51962833952958043</v>
+      </c>
+      <c r="D41">
+        <v>3.2159805150617622</v>
+      </c>
+      <c r="E41">
+        <v>5.912332690593944</v>
+      </c>
+      <c r="F41">
+        <v>1.8037341275633167E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <v>-1.4664648033161805</v>
+      </c>
+      <c r="D42">
+        <v>2.3131557246141377</v>
+      </c>
+      <c r="E42">
+        <v>6.0927762525444553</v>
+      </c>
+      <c r="F42">
+        <v>0.28893155650949209</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" t="s">
+        <v>21</v>
+      </c>
+      <c r="F45" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46">
+        <v>332.04051728202421</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>166.02025864101211</v>
+      </c>
+      <c r="E46">
+        <v>4.4029412458214754</v>
+      </c>
+      <c r="F46">
+        <v>2.6844833809628543E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47">
+        <v>716.42675613099232</v>
+      </c>
+      <c r="C47">
+        <v>19</v>
+      </c>
+      <c r="D47">
+        <v>37.706671375315388</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48">
+        <v>1048.4672734130165</v>
+      </c>
+      <c r="C48">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>27</v>
+      </c>
+      <c r="B51" t="s">
+        <v>27</v>
+      </c>
+      <c r="F51" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <v>-21.285164165472565</v>
+      </c>
+      <c r="D52">
+        <v>-11.360413609621634</v>
+      </c>
+      <c r="E52">
+        <v>-1.4356630537707016</v>
+      </c>
+      <c r="F52">
+        <v>2.3398736229205741E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <v>-8.2845119578637618</v>
+      </c>
+      <c r="D53">
+        <v>-0.15718811283753276</v>
+      </c>
+      <c r="E53">
+        <v>7.9701357321886963</v>
+      </c>
+      <c r="F53">
+        <v>0.99866999106135879</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>2</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="C54">
+        <v>-0.18927742644246592</v>
+      </c>
+      <c r="D54">
+        <v>11.203225496784102</v>
+      </c>
+      <c r="E54">
+        <v>22.595728420010669</v>
+      </c>
+      <c r="F54">
+        <v>5.4406741867658259E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>